<commit_message>
Experimentos finalizados; ResultsControl em processo de atualização, agora com o desvio padrão de cada média geral; Alguns experimentos estão sendo refeitos, devido a mudanças que ocorreram depois; A leitura de arquivos xlsx no MAC OSX não funciona quando a célula lida possui fórmula (a não ser que o Excel seja aberto e os campos sejam recalculados).
</commit_message>
<xml_diff>
--- a/PaperNeural/Results/ResultsMar2017-Empty.xlsx
+++ b/PaperNeural/Results/ResultsMar2017-Empty.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliveirafhm/Dropbox/Compartilhada Alessando e Fabio/Clinic 09.03.2016/Programs/oliveirafhm/PaperNeural/Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliveirafhm/Dropbox/Compartilhada Alessando e Fabio/Clinic 09.03.2016/Programs/oliveirafhm/code_paper_journal_2017/PaperNeural/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="50">
   <si>
     <t>Class</t>
   </si>
@@ -631,9 +631,6 @@
   </si>
   <si>
     <t>SDBS</t>
-  </si>
-  <si>
-    <t>General mean</t>
   </si>
   <si>
     <t>OK</t>
@@ -1511,20 +1508,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="M64" sqref="M64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="8.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.83203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="13" width="9.33203125" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="22" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="9.5" customWidth="1"/>
@@ -1537,7 +1537,7 @@
         <v>33</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -5770,7 +5770,7 @@
         <v>18</v>
       </c>
       <c r="O49" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P49" t="s">
         <v>18</v>
@@ -6603,7 +6603,7 @@
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.2">
       <c r="P65" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.2">
@@ -6772,86 +6772,124 @@
       </c>
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A72" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="B72" s="54"/>
+      <c r="C72" s="51" t="str">
+        <f t="shared" ref="C72:K72" si="95">C2</f>
+        <v>SH (SH)</v>
+      </c>
+      <c r="D72" s="49" t="str">
+        <f t="shared" si="95"/>
+        <v>SH (SPD)</v>
+      </c>
+      <c r="E72" s="49" t="str">
+        <f t="shared" si="95"/>
+        <v>SH (SDBS)</v>
+      </c>
+      <c r="F72" s="50" t="str">
+        <f t="shared" si="95"/>
+        <v>SPD (SH)</v>
+      </c>
+      <c r="G72" s="50" t="str">
+        <f t="shared" si="95"/>
+        <v>SPD (SPD)</v>
+      </c>
+      <c r="H72" s="49" t="str">
+        <f t="shared" si="95"/>
+        <v>SPD (SDBS)</v>
+      </c>
+      <c r="I72" s="49" t="str">
+        <f t="shared" si="95"/>
+        <v>SDBS (SH)</v>
+      </c>
+      <c r="J72" s="49" t="str">
+        <f t="shared" si="95"/>
+        <v>SDBS (SPD)</v>
+      </c>
+      <c r="K72" s="49" t="str">
+        <f t="shared" si="95"/>
+        <v>SDBS (SDBS)</v>
+      </c>
       <c r="O72" s="53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P72" s="54"/>
       <c r="Q72" s="51" t="str">
-        <f t="shared" ref="Q72:Y72" si="95">Q2</f>
+        <f t="shared" ref="Q72:Y72" si="96">Q2</f>
         <v>SH (SH)</v>
       </c>
       <c r="R72" s="49" t="str">
-        <f t="shared" si="95"/>
+        <f t="shared" si="96"/>
         <v>SH (SPD)</v>
       </c>
       <c r="S72" s="49" t="str">
-        <f t="shared" si="95"/>
+        <f t="shared" si="96"/>
         <v>SH (SDBS)</v>
       </c>
       <c r="T72" s="50" t="str">
-        <f t="shared" si="95"/>
+        <f t="shared" si="96"/>
         <v>SPD (SH)</v>
       </c>
       <c r="U72" s="50" t="str">
-        <f t="shared" si="95"/>
+        <f t="shared" si="96"/>
         <v>SPD (SPD)</v>
       </c>
       <c r="V72" s="49" t="str">
-        <f t="shared" si="95"/>
+        <f t="shared" si="96"/>
         <v>SPD (SDBS)</v>
       </c>
       <c r="W72" s="49" t="str">
-        <f t="shared" si="95"/>
+        <f t="shared" si="96"/>
         <v>SDBS (SH)</v>
       </c>
       <c r="X72" s="49" t="str">
-        <f t="shared" si="95"/>
+        <f t="shared" si="96"/>
         <v>SDBS (SPD)</v>
       </c>
       <c r="Y72" s="49" t="str">
-        <f t="shared" si="95"/>
+        <f t="shared" si="96"/>
         <v>SDBS (SDBS)</v>
       </c>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>41</v>
-      </c>
-      <c r="B73" s="39"/>
+      <c r="A73" s="46"/>
+      <c r="B73" s="52"/>
       <c r="C73" s="36" t="e">
         <f>AVERAGE(C7,C13,C19,C25,C31,C37,C43)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D73" s="35" t="e">
-        <f t="shared" ref="D73:K73" si="96">AVERAGE(D7,D13,D19,D25,D31,D37,D43)</f>
+        <f t="shared" ref="D73:K73" si="97">AVERAGE(D7,D13,D19,D25,D31,D37,D43)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E73" s="35" t="e">
-        <f t="shared" si="96"/>
+        <f t="shared" si="97"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F73" s="35" t="e">
-        <f t="shared" si="96"/>
+        <f t="shared" si="97"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G73" s="36" t="e">
-        <f t="shared" si="96"/>
+        <f t="shared" si="97"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H73" s="35" t="e">
-        <f t="shared" si="96"/>
+        <f t="shared" si="97"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I73" s="35" t="e">
-        <f t="shared" si="96"/>
+        <f t="shared" si="97"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J73" s="39" t="e">
-        <f t="shared" si="96"/>
+        <f t="shared" si="97"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K73" s="36" t="e">
-        <f t="shared" si="96"/>
+        <f t="shared" si="97"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L73" s="35"/>
@@ -6863,125 +6901,123 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R73" s="35" t="e">
-        <f t="shared" ref="R73:Y74" si="97">AVERAGE(R7,R13,R19,R25,R31,R37,R43)</f>
+        <f t="shared" ref="R73:Y74" si="98">AVERAGE(R7,R13,R19,R25,R31,R37,R43)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S73" s="35" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="98"/>
         <v>#DIV/0!</v>
       </c>
       <c r="T73" s="35" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="98"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U73" s="36" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="98"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V73" s="35" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="98"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W73" s="35" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="98"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X73" s="39" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="98"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y73" s="36" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="98"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A74" s="46"/>
+      <c r="B74" s="46" t="s">
+        <v>45</v>
+      </c>
       <c r="C74" s="35" t="e">
         <f>AVERAGE(C8,C14,C20,C26,C32,C38,C44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D74" s="35" t="e">
-        <f t="shared" ref="D74:K74" si="98">AVERAGE(D8,D14,D20,D26,D32,D38,D44)</f>
+        <f t="shared" ref="D74:K74" si="99">AVERAGE(D8,D14,D20,D26,D32,D38,D44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E74" s="35" t="e">
-        <f t="shared" si="98"/>
+        <f t="shared" si="99"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F74" s="35" t="e">
-        <f t="shared" si="98"/>
+        <f t="shared" si="99"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G74" s="35" t="e">
-        <f t="shared" si="98"/>
+        <f t="shared" si="99"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H74" s="35" t="e">
-        <f t="shared" si="98"/>
+        <f t="shared" si="99"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I74" s="35" t="e">
-        <f t="shared" si="98"/>
+        <f t="shared" si="99"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J74" s="35" t="e">
-        <f t="shared" si="98"/>
+        <f t="shared" si="99"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K74" s="35" t="e">
-        <f t="shared" si="98"/>
+        <f t="shared" si="99"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O74" s="46"/>
       <c r="P74" s="46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q74" s="35" t="e">
         <f>AVERAGE(Q8,Q14,Q20,Q26,Q32,Q38,Q44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R74" s="35" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="98"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S74" s="35" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="98"/>
         <v>#DIV/0!</v>
       </c>
       <c r="T74" s="35" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="98"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U74" s="35" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="98"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V74" s="35" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="98"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W74" s="35" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="98"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X74" s="35" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="98"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y74" s="35" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="98"/>
         <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="A39:A44"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="A21:A26"/>
+  <mergeCells count="16">
+    <mergeCell ref="A72:B72"/>
     <mergeCell ref="O72:P72"/>
     <mergeCell ref="O33:O38"/>
     <mergeCell ref="O39:O44"/>
@@ -6990,6 +7026,13 @@
     <mergeCell ref="O15:O20"/>
     <mergeCell ref="O21:O26"/>
     <mergeCell ref="O27:O32"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A21:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -7003,8 +7046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="N4" activeCellId="3" sqref="N22:N23 N16:N17 N10:N11 N4:N5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7018,7 +7061,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -7054,7 +7097,7 @@
         <v>6</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
@@ -7067,7 +7110,7 @@
         <v>6</v>
       </c>
       <c r="N4" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -7196,7 +7239,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="63" t="s">
@@ -7208,7 +7251,7 @@
         <v>6</v>
       </c>
       <c r="N10" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -7330,7 +7373,7 @@
         <v>6</v>
       </c>
       <c r="G16" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="63" t="s">
@@ -7342,7 +7385,7 @@
         <v>6</v>
       </c>
       <c r="N16" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -7464,7 +7507,7 @@
         <v>6</v>
       </c>
       <c r="G22" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="63" t="s">
@@ -7476,7 +7519,7 @@
         <v>6</v>
       </c>
       <c r="N22" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="32" customHeight="1" x14ac:dyDescent="0.2">
@@ -7637,8 +7680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="N4" activeCellId="3" sqref="N22:N23 N16:N17 N10:N11 N4:N5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7652,7 +7695,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -7688,7 +7731,7 @@
         <v>6</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="2"/>
@@ -7701,7 +7744,7 @@
         <v>6</v>
       </c>
       <c r="N4" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -7827,7 +7870,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="63" t="s">
@@ -7839,7 +7882,7 @@
         <v>6</v>
       </c>
       <c r="N10" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -7961,7 +8004,7 @@
         <v>6</v>
       </c>
       <c r="G16" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="63" t="s">
@@ -7973,7 +8016,7 @@
         <v>6</v>
       </c>
       <c r="N16" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -8095,7 +8138,7 @@
         <v>6</v>
       </c>
       <c r="G22" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="63" t="s">
@@ -8107,7 +8150,7 @@
         <v>6</v>
       </c>
       <c r="N22" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="32" customHeight="1" x14ac:dyDescent="0.2">
@@ -8268,8 +8311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="N4" activeCellId="3" sqref="N22:N23 N16:N17 N10:N11 N4:N5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8283,7 +8326,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -8319,7 +8362,7 @@
         <v>6</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="2"/>
@@ -8332,7 +8375,7 @@
         <v>6</v>
       </c>
       <c r="N4" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -8458,7 +8501,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="63" t="s">
@@ -8470,7 +8513,7 @@
         <v>6</v>
       </c>
       <c r="N10" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -8592,7 +8635,7 @@
         <v>6</v>
       </c>
       <c r="G16" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="63" t="s">
@@ -8604,7 +8647,7 @@
         <v>6</v>
       </c>
       <c r="N16" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -8726,7 +8769,7 @@
         <v>6</v>
       </c>
       <c r="G22" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="63" t="s">
@@ -8738,7 +8781,7 @@
         <v>6</v>
       </c>
       <c r="N22" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="32" customHeight="1" x14ac:dyDescent="0.2">
@@ -8899,8 +8942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="N22" activeCellId="3" sqref="N4:N5 N10:N11 N16:N17 N22:N23"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8914,7 +8957,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -8950,7 +8993,7 @@
         <v>6</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="2"/>
@@ -8963,7 +9006,7 @@
         <v>6</v>
       </c>
       <c r="N4" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -9089,7 +9132,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="63" t="s">
@@ -9101,7 +9144,7 @@
         <v>6</v>
       </c>
       <c r="N10" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -9223,7 +9266,7 @@
         <v>6</v>
       </c>
       <c r="G16" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="63" t="s">
@@ -9235,7 +9278,7 @@
         <v>6</v>
       </c>
       <c r="N16" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -9357,7 +9400,7 @@
         <v>6</v>
       </c>
       <c r="G22" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="63" t="s">
@@ -9369,7 +9412,7 @@
         <v>6</v>
       </c>
       <c r="N22" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="32" customHeight="1" x14ac:dyDescent="0.2">
@@ -9529,8 +9572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G22" activeCellId="2" sqref="G10:G11 G16:G17 G22:G23"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9577,7 +9620,7 @@
         <v>6</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" s="42"/>
       <c r="I4" s="41"/>
@@ -9590,7 +9633,7 @@
         <v>6</v>
       </c>
       <c r="N4" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -9716,7 +9759,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I10" s="41"/>
       <c r="J10" s="63" t="s">
@@ -9728,7 +9771,7 @@
         <v>6</v>
       </c>
       <c r="N10" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -9850,7 +9893,7 @@
         <v>6</v>
       </c>
       <c r="G16" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="63" t="s">
@@ -9862,7 +9905,7 @@
         <v>6</v>
       </c>
       <c r="N16" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -9984,7 +10027,7 @@
         <v>6</v>
       </c>
       <c r="G22" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="63" t="s">
@@ -9996,7 +10039,7 @@
         <v>6</v>
       </c>
       <c r="N22" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="32" customHeight="1" x14ac:dyDescent="0.2">
@@ -10157,8 +10200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G22" activeCellId="3" sqref="G4:G5 G10:G11 G16:G17 G22:G23"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10172,7 +10215,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -10208,7 +10251,7 @@
         <v>6</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" s="42"/>
       <c r="I4" s="41"/>
@@ -10221,7 +10264,7 @@
         <v>6</v>
       </c>
       <c r="N4" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -10347,7 +10390,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I10" s="41"/>
       <c r="J10" s="63" t="s">
@@ -10359,7 +10402,7 @@
         <v>6</v>
       </c>
       <c r="N10" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -10481,7 +10524,7 @@
         <v>6</v>
       </c>
       <c r="G16" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I16" s="41"/>
       <c r="J16" s="63" t="s">
@@ -10493,7 +10536,7 @@
         <v>6</v>
       </c>
       <c r="N16" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -10615,7 +10658,7 @@
         <v>6</v>
       </c>
       <c r="G22" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I22" s="41"/>
       <c r="J22" s="63" t="s">
@@ -10627,7 +10670,7 @@
         <v>6</v>
       </c>
       <c r="N22" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="32" customHeight="1" x14ac:dyDescent="0.2">
@@ -10803,7 +10846,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -10839,7 +10882,7 @@
         <v>6</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" s="42"/>
       <c r="I4" s="41"/>
@@ -10852,7 +10895,7 @@
         <v>6</v>
       </c>
       <c r="N4" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P4" s="44"/>
       <c r="Q4" s="44"/>
@@ -10987,7 +11030,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I10" s="41"/>
       <c r="J10" s="63" t="s">
@@ -10999,7 +11042,7 @@
         <v>6</v>
       </c>
       <c r="N10" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -11121,7 +11164,7 @@
         <v>6</v>
       </c>
       <c r="G16" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I16" s="41"/>
       <c r="J16" s="63" t="s">
@@ -11133,7 +11176,7 @@
         <v>6</v>
       </c>
       <c r="N16" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -11255,7 +11298,7 @@
         <v>6</v>
       </c>
       <c r="G22" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I22" s="41"/>
       <c r="J22" s="63" t="s">
@@ -11267,7 +11310,7 @@
         <v>6</v>
       </c>
       <c r="N22" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="32" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>